<commit_message>
Save work: add correos flow, CLIENTES, fixes and tests passing
</commit_message>
<xml_diff>
--- a/BD/PREPAGOS.XLSX
+++ b/BD/PREPAGOS.XLSX
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gorderiquev\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BCP DIARIO\2026\FEBRERO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{365B5DC1-157E-417D-92BD-927F9F6C68A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8BE1985-DA72-488F-835D-41E18C52789A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{35086493-8F9D-4967-AE5C-7F4699DBE20D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EF5E465E-0458-4A43-887C-EF459EF79701}"/>
   </bookViews>
   <sheets>
     <sheet name="PREPAGOS" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="656">
   <si>
     <t>DIAZ VALIENTE, ROSALIA</t>
   </si>
@@ -1999,13 +1999,16 @@
   </si>
   <si>
     <t>VERGARA AGUINAGA OSCAR ALFONSO</t>
+  </si>
+  <si>
+    <t>Clavijo Salazar, Luz Milagros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2026,16 +2029,28 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2073,12 +2088,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -2092,10 +2131,16 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2 2" xfId="1" xr:uid="{678E6111-C440-4A24-B48E-BACA2D7F4FB8}"/>
+    <cellStyle name="Normal 2 2 2" xfId="1" xr:uid="{881D2160-EFF8-4CA9-9E78-6A70E1D7549C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2406,146 +2451,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE407A0-7E43-4C30-8D09-051F553B6995}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE90BB6E-4032-444D-A47D-2F971C570C45}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:B757"/>
+  <dimension ref="A1:B758"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+    <sheetView tabSelected="1" topLeftCell="A737" workbookViewId="0">
+      <selection activeCell="A442" sqref="A442:A758"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="9" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="513" max="513" width="9" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="769" max="769" width="9" bestFit="1" customWidth="1"/>
-    <col min="770" max="770" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="1025" max="1025" width="9" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1026" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="1281" max="1281" width="9" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1282" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="1537" max="1537" width="9" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1538" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="1793" max="1793" width="9" bestFit="1" customWidth="1"/>
-    <col min="1794" max="1794" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="2049" max="2049" width="9" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2050" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="2305" max="2305" width="9" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2306" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="2561" max="2561" width="9" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2562" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="2817" max="2817" width="9" bestFit="1" customWidth="1"/>
-    <col min="2818" max="2818" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3073" max="3073" width="9" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3074" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3329" max="3329" width="9" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3330" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3585" max="3585" width="9" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3586" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3841" max="3841" width="9" bestFit="1" customWidth="1"/>
-    <col min="3842" max="3842" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="4097" max="4097" width="9" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4098" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="4353" max="4353" width="9" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4354" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="4609" max="4609" width="9" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4610" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="4865" max="4865" width="9" bestFit="1" customWidth="1"/>
-    <col min="4866" max="4866" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="5121" max="5121" width="9" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5122" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="5377" max="5377" width="9" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5378" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="5633" max="5633" width="9" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5634" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="5889" max="5889" width="9" bestFit="1" customWidth="1"/>
-    <col min="5890" max="5890" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="6145" max="6145" width="9" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6146" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="6401" max="6401" width="9" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6402" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="6657" max="6657" width="9" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6658" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="6913" max="6913" width="9" bestFit="1" customWidth="1"/>
-    <col min="6914" max="6914" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="7169" max="7169" width="9" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7170" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="7425" max="7425" width="9" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7426" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="7681" max="7681" width="9" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7682" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="7937" max="7937" width="9" bestFit="1" customWidth="1"/>
-    <col min="7938" max="7938" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="8193" max="8193" width="9" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8194" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="8449" max="8449" width="9" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8450" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="8705" max="8705" width="9" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8706" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="8961" max="8961" width="9" bestFit="1" customWidth="1"/>
-    <col min="8962" max="8962" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="9217" max="9217" width="9" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9218" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="9473" max="9473" width="9" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9474" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="9729" max="9729" width="9" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9730" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="9985" max="9985" width="9" bestFit="1" customWidth="1"/>
-    <col min="9986" max="9986" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="10241" max="10241" width="9" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10242" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="10497" max="10497" width="9" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10498" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="10753" max="10753" width="9" bestFit="1" customWidth="1"/>
-    <col min="10754" max="10754" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="11009" max="11009" width="9" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11010" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="11265" max="11265" width="9" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11266" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="11521" max="11521" width="9" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11522" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="11777" max="11777" width="9" bestFit="1" customWidth="1"/>
-    <col min="11778" max="11778" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="12033" max="12033" width="9" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12034" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="12289" max="12289" width="9" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12290" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="12545" max="12545" width="9" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12546" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="12801" max="12801" width="9" bestFit="1" customWidth="1"/>
-    <col min="12802" max="12802" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="13057" max="13057" width="9" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="13313" max="13313" width="9" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13314" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="13569" max="13569" width="9" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13570" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="13825" max="13825" width="9" bestFit="1" customWidth="1"/>
-    <col min="13826" max="13826" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="14081" max="14081" width="9" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14082" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="14337" max="14337" width="9" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14338" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="14593" max="14593" width="9" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14594" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="14849" max="14849" width="9" bestFit="1" customWidth="1"/>
-    <col min="14850" max="14850" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="15105" max="15105" width="9" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15106" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="15361" max="15361" width="9" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15362" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="15617" max="15617" width="9" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15618" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="15873" max="15873" width="9" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15874" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="16129" max="16129" width="9" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16130" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="256" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -8604,6 +8524,14 @@
         <v>654</v>
       </c>
     </row>
+    <row r="758" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A758" s="4">
+        <v>36918110</v>
+      </c>
+      <c r="B758" s="5" t="s">
+        <v>655</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: implementación de sistema de envío de correos electrónicos
</commit_message>
<xml_diff>
--- a/BD/PREPAGOS.XLSX
+++ b/BD/PREPAGOS.XLSX
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gorderiquev\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BCP DIARIO\2026\FEBRERO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{365B5DC1-157E-417D-92BD-927F9F6C68A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8BE1985-DA72-488F-835D-41E18C52789A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{35086493-8F9D-4967-AE5C-7F4699DBE20D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EF5E465E-0458-4A43-887C-EF459EF79701}"/>
   </bookViews>
   <sheets>
     <sheet name="PREPAGOS" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="656">
   <si>
     <t>DIAZ VALIENTE, ROSALIA</t>
   </si>
@@ -1999,13 +1999,16 @@
   </si>
   <si>
     <t>VERGARA AGUINAGA OSCAR ALFONSO</t>
+  </si>
+  <si>
+    <t>Clavijo Salazar, Luz Milagros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2026,16 +2029,28 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2073,12 +2088,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -2092,10 +2131,16 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2 2" xfId="1" xr:uid="{678E6111-C440-4A24-B48E-BACA2D7F4FB8}"/>
+    <cellStyle name="Normal 2 2 2" xfId="1" xr:uid="{881D2160-EFF8-4CA9-9E78-6A70E1D7549C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2406,146 +2451,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE407A0-7E43-4C30-8D09-051F553B6995}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE90BB6E-4032-444D-A47D-2F971C570C45}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:B757"/>
+  <dimension ref="A1:B758"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+    <sheetView tabSelected="1" topLeftCell="A737" workbookViewId="0">
+      <selection activeCell="A442" sqref="A442:A758"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="9" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="513" max="513" width="9" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="769" max="769" width="9" bestFit="1" customWidth="1"/>
-    <col min="770" max="770" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="1025" max="1025" width="9" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1026" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="1281" max="1281" width="9" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1282" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="1537" max="1537" width="9" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1538" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="1793" max="1793" width="9" bestFit="1" customWidth="1"/>
-    <col min="1794" max="1794" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="2049" max="2049" width="9" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2050" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="2305" max="2305" width="9" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2306" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="2561" max="2561" width="9" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2562" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="2817" max="2817" width="9" bestFit="1" customWidth="1"/>
-    <col min="2818" max="2818" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3073" max="3073" width="9" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3074" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3329" max="3329" width="9" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3330" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3585" max="3585" width="9" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3586" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3841" max="3841" width="9" bestFit="1" customWidth="1"/>
-    <col min="3842" max="3842" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="4097" max="4097" width="9" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4098" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="4353" max="4353" width="9" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4354" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="4609" max="4609" width="9" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4610" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="4865" max="4865" width="9" bestFit="1" customWidth="1"/>
-    <col min="4866" max="4866" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="5121" max="5121" width="9" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5122" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="5377" max="5377" width="9" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5378" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="5633" max="5633" width="9" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5634" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="5889" max="5889" width="9" bestFit="1" customWidth="1"/>
-    <col min="5890" max="5890" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="6145" max="6145" width="9" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6146" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="6401" max="6401" width="9" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6402" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="6657" max="6657" width="9" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6658" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="6913" max="6913" width="9" bestFit="1" customWidth="1"/>
-    <col min="6914" max="6914" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="7169" max="7169" width="9" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7170" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="7425" max="7425" width="9" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7426" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="7681" max="7681" width="9" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7682" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="7937" max="7937" width="9" bestFit="1" customWidth="1"/>
-    <col min="7938" max="7938" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="8193" max="8193" width="9" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8194" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="8449" max="8449" width="9" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8450" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="8705" max="8705" width="9" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8706" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="8961" max="8961" width="9" bestFit="1" customWidth="1"/>
-    <col min="8962" max="8962" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="9217" max="9217" width="9" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9218" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="9473" max="9473" width="9" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9474" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="9729" max="9729" width="9" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9730" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="9985" max="9985" width="9" bestFit="1" customWidth="1"/>
-    <col min="9986" max="9986" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="10241" max="10241" width="9" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10242" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="10497" max="10497" width="9" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10498" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="10753" max="10753" width="9" bestFit="1" customWidth="1"/>
-    <col min="10754" max="10754" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="11009" max="11009" width="9" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11010" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="11265" max="11265" width="9" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11266" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="11521" max="11521" width="9" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11522" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="11777" max="11777" width="9" bestFit="1" customWidth="1"/>
-    <col min="11778" max="11778" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="12033" max="12033" width="9" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12034" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="12289" max="12289" width="9" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12290" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="12545" max="12545" width="9" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12546" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="12801" max="12801" width="9" bestFit="1" customWidth="1"/>
-    <col min="12802" max="12802" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="13057" max="13057" width="9" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="13313" max="13313" width="9" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13314" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="13569" max="13569" width="9" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13570" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="13825" max="13825" width="9" bestFit="1" customWidth="1"/>
-    <col min="13826" max="13826" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="14081" max="14081" width="9" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14082" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="14337" max="14337" width="9" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14338" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="14593" max="14593" width="9" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14594" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="14849" max="14849" width="9" bestFit="1" customWidth="1"/>
-    <col min="14850" max="14850" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="15105" max="15105" width="9" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15106" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="15361" max="15361" width="9" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15362" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="15617" max="15617" width="9" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15618" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="15873" max="15873" width="9" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15874" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="16129" max="16129" width="9" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16130" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="256" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -8604,6 +8524,14 @@
         <v>654</v>
       </c>
     </row>
+    <row r="758" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A758" s="4">
+        <v>36918110</v>
+      </c>
+      <c r="B758" s="5" t="s">
+        <v>655</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>